<commit_message>
Configure line endings for pgbouncer-config.sh
</commit_message>
<xml_diff>
--- a/assets/options.xlsx
+++ b/assets/options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/julius_schlumberger_deltares_nl/Documents/Documents/NWL/votingPlatform/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_F25DC773A252ABDACC10486EE99A6A045BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{049B3550-BF40-42A0-A29B-638BDA0B964D}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="11_F25DC773A252ABDACC10486EE99A6A045BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD29A37C-E413-4638-B0A5-69B92748DEAE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>Contributie in valuta èn natura als basis</t>
   </si>
@@ -73,6 +73,129 @@
   </si>
   <si>
     <t>Aanpassen aan huurprijzen van vergelijkbare voormalige kraakpanden in de omgeving</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>#c2e6f5</t>
+  </si>
+  <si>
+    <t>#8bd3fa</t>
+  </si>
+  <si>
+    <t>#4ebdff</t>
+  </si>
+  <si>
+    <t>#00a6ff</t>
+  </si>
+  <si>
+    <t>#008ff9</t>
+  </si>
+  <si>
+    <t>#007ae3</t>
+  </si>
+  <si>
+    <t>#0063d7</t>
+  </si>
+  <si>
+    <t>#001aff</t>
+  </si>
+  <si>
+    <t>#c2f5c2</t>
+  </si>
+  <si>
+    <t>#84fc7f</t>
+  </si>
+  <si>
+    <t>#05ff00</t>
+  </si>
+  <si>
+    <t>#453e03</t>
+  </si>
+  <si>
+    <t>#7c6e04</t>
+  </si>
+  <si>
+    <t>#bba103</t>
+  </si>
+  <si>
+    <t>#ffd600</t>
+  </si>
+  <si>
+    <t>Colors2</t>
+  </si>
+  <si>
+    <t>#ffcc33</t>
+  </si>
+  <si>
+    <t>#1159d5</t>
+  </si>
+  <si>
+    <t>#1467f7</t>
+  </si>
+  <si>
+    <t>#4a8af7</t>
+  </si>
+  <si>
+    <t>#6fa1f7</t>
+  </si>
+  <si>
+    <t>#8fb6f7</t>
+  </si>
+  <si>
+    <t>#adc8f7</t>
+  </si>
+  <si>
+    <t>#dae5f7</t>
+  </si>
+  <si>
+    <t>#f54949</t>
+  </si>
+  <si>
+    <t>#f4cccc</t>
+  </si>
+  <si>
+    <t>#ffe9a6</t>
+  </si>
+  <si>
+    <t>#fff5d9</t>
+  </si>
+  <si>
+    <t>#ffb300</t>
+  </si>
+  <si>
+    <t>#f57676</t>
+  </si>
+  <si>
+    <t>#f5a2a2</t>
+  </si>
+  <si>
+    <t>Colors3</t>
+  </si>
+  <si>
+    <t>#ff0000</t>
+  </si>
+  <si>
+    <t>#ff6573</t>
+  </si>
+  <si>
+    <t>#f2a6b8</t>
+  </si>
+  <si>
+    <t>#ffc800</t>
+  </si>
+  <si>
+    <t>#ffedad</t>
+  </si>
+  <si>
+    <t>#ffe181</t>
+  </si>
+  <si>
+    <t>#ffd552</t>
   </si>
 </sst>
 </file>
@@ -108,7 +231,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,7 +240,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,21 +284,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,99 +584,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="111" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="111" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="1" t="s">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
+      <c r="B7" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="1">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
+      <c r="B10" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="1" t="s">
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+      <c r="B13" s="1">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="B14" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="B15" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>